<commit_message>
Update Project Cost projections.xlsx
</commit_message>
<xml_diff>
--- a/Progress Report/Project Cost projections.xlsx
+++ b/Progress Report/Project Cost projections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Desktop\Fifth Year\Winter\SYSC 4805\Project\SYSC4805\Progress Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ADB7A3-BE76-4600-B29B-F209077F1093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE3BDA6-5B28-4854-9C95-5BE6CF8F1964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="525" windowWidth="18210" windowHeight="20220" xr2:uid="{8D004C25-59CC-4F99-8D52-27451170976B}"/>
+    <workbookView xWindow="18300" yWindow="390" windowWidth="18210" windowHeight="20220" xr2:uid="{8D004C25-59CC-4F99-8D52-27451170976B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>3D printer fillament</t>
   </si>
   <si>
-    <t>https://www.amazon.ca/DURAMIC-3D-Filament-1-75mm-Black-1/dp/B095HRG913/ref=sr_1_2_sspa?keywords=3d+printing+filament&amp;qid=1646089701&amp;sprefix=3d+printing+fil%2Caps%2C108&amp;sr=8-2-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzM0ozUlNGTDVVSEhKJmVuY3J5cHRlZElkPUEwNzk0MDAyM0QxVEgwUDBQTzFBTiZlbmNyeXB0ZWRBZElkPUEwOTA2OTkyMjlQUUszOUZNVUhIRSZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=</t>
-  </si>
-  <si>
     <t>Total Materials Cost</t>
   </si>
   <si>
@@ -113,6 +110,9 @@
   </si>
   <si>
     <t>Total Projected Cost</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/DURAMIC-3D-Filament-1-75mm-Black-1/dp/B095HRG913/ref=sr_1_2_sspa?keywords=3d+printing+filament&amp;qid=1646089701&amp;sprefix=3d+printing+fil%2Caps%2C108&amp;sr=8-2-spons&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331D1329-9C45-4A3B-9A57-04555DEDFED7}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <f>4*4</f>
+        <f t="shared" ref="C2:C8" si="0">4*4</f>
         <v>16</v>
       </c>
       <c r="D2">
@@ -573,7 +573,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <f>4*4</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D3">
@@ -581,7 +581,7 @@
         <v>400</v>
       </c>
       <c r="E3">
-        <f>E2+D3</f>
+        <f t="shared" ref="E3:E8" si="1">E2+D3</f>
         <v>800</v>
       </c>
       <c r="G3" t="s">
@@ -609,7 +609,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <f>4*4</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D4">
@@ -617,7 +617,7 @@
         <v>400</v>
       </c>
       <c r="E4">
-        <f>E3+D4</f>
+        <f t="shared" si="1"/>
         <v>1200</v>
       </c>
       <c r="G4" t="s">
@@ -645,7 +645,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <f>4*4</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D5">
@@ -653,7 +653,7 @@
         <v>400</v>
       </c>
       <c r="E5">
-        <f>E4+D5</f>
+        <f t="shared" si="1"/>
         <v>1600</v>
       </c>
       <c r="G5" t="s">
@@ -670,7 +670,7 @@
         <v>35</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -681,7 +681,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <f>4*4</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D6">
@@ -689,11 +689,11 @@
         <v>400</v>
       </c>
       <c r="E6">
-        <f>E5+D6</f>
+        <f t="shared" si="1"/>
         <v>2000</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -707,7 +707,7 @@
         <v>650</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <f>4*4</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D7">
@@ -726,7 +726,7 @@
         <v>400</v>
       </c>
       <c r="E7">
-        <f>E6+D7</f>
+        <f t="shared" si="1"/>
         <v>2400</v>
       </c>
     </row>
@@ -738,7 +738,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <f>4*4</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D8">
@@ -746,7 +746,7 @@
         <v>400</v>
       </c>
       <c r="E8">
-        <f>E7+D8</f>
+        <f t="shared" si="1"/>
         <v>2800</v>
       </c>
     </row>
@@ -758,13 +758,13 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J11">
         <f>SUM(J2:J8)</f>
@@ -799,5 +799,6 @@
     <hyperlink ref="K6" r:id="rId4" xr:uid="{1CFF1102-BF7D-4A76-89FD-2F4A6E5F1ACF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>